<commit_message>
Listo alta de alumnos
</commit_message>
<xml_diff>
--- a/proyecto/media/Prueba Excel.xlsx
+++ b/proyecto/media/Prueba Excel.xlsx
@@ -1,7 +1,7 @@
 
 <file path=META-INF/manifest.xml><?xml version="1.0" encoding="utf-8"?>
-<manifest:manifest xmlns:manifest="urn:oasis:names:tc:opendocument:xmlns:manifest:1.0" xmlns:loext="urn:org:documentfoundation:names:experimental:office:xmlns:loext:1.0" manifest:version="1.2">
-  <manifest:file-entry manifest:full-path="/" manifest:version="1.2" manifest:media-type="application/vnd.oasis.opendocument.spreadsheet"/>
+<manifest:manifest xmlns:manifest="urn:oasis:names:tc:opendocument:xmlns:manifest:1.0" xmlns:loext="urn:org:documentfoundation:names:experimental:office:xmlns:loext:1.0" manifest:version="1.3">
+  <manifest:file-entry manifest:full-path="/" manifest:version="1.3" manifest:media-type="application/vnd.oasis.opendocument.spreadsheet"/>
   <manifest:file-entry manifest:full-path="Configurations2/" manifest:media-type="application/vnd.sun.xml.ui.configuration"/>
   <manifest:file-entry manifest:full-path="manifest.rdf" manifest:media-type="application/rdf+xml"/>
   <manifest:file-entry manifest:full-path="meta.xml" manifest:media-type="text/xml"/>
@@ -13,23 +13,23 @@
 </file>
 
 <file path=content.xml><?xml version="1.0" encoding="utf-8"?>
-<office:document-content xmlns:presentation="urn:oasis:names:tc:opendocument:xmlns:presentation:1.0" xmlns:css3t="http://www.w3.org/TR/css3-text/" xmlns:grddl="http://www.w3.org/2003/g/data-view#" xmlns:xhtml="http://www.w3.org/1999/xhtml" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:chart="urn:oasis:names:tc:opendocument:xmlns:chart:1.0" xmlns:svg="urn:oasis:names:tc:opendocument:xmlns:svg-compatible:1.0" xmlns:draw="urn:oasis:names:tc:opendocument:xmlns:drawing:1.0" xmlns:rpt="http://openoffice.org/2005/report" xmlns:text="urn:oasis:names:tc:opendocument:xmlns:text:1.0" xmlns:style="urn:oasis:names:tc:opendocument:xmlns:style:1.0" xmlns:meta="urn:oasis:names:tc:opendocument:xmlns:meta:1.0" xmlns:xlink="http://www.w3.org/1999/xlink" xmlns:fo="urn:oasis:names:tc:opendocument:xmlns:xsl-fo-compatible:1.0" xmlns:of="urn:oasis:names:tc:opendocument:xmlns:of:1.2" xmlns:dc="http://purl.org/dc/elements/1.1/" xmlns:ooo="http://openoffice.org/2004/office" xmlns:dr3d="urn:oasis:names:tc:opendocument:xmlns:dr3d:1.0" xmlns:formx="urn:openoffice:names:experimental:ooxml-odf-interop:xmlns:form:1.0" xmlns:calcext="urn:org:documentfoundation:names:experimental:calc:xmlns:calcext:1.0" xmlns:drawooo="http://openoffice.org/2010/draw" xmlns:field="urn:openoffice:names:experimental:ooo-ms-interop:xmlns:field:1.0" xmlns:office="urn:oasis:names:tc:opendocument:xmlns:office:1.0" xmlns:table="urn:oasis:names:tc:opendocument:xmlns:table:1.0" xmlns:number="urn:oasis:names:tc:opendocument:xmlns:datastyle:1.0" xmlns:ooow="http://openoffice.org/2004/writer" xmlns:oooc="http://openoffice.org/2004/calc" xmlns:tableooo="http://openoffice.org/2009/table" xmlns:loext="urn:org:documentfoundation:names:experimental:office:xmlns:loext:1.0" xmlns:math="http://www.w3.org/1998/Math/MathML" xmlns:form="urn:oasis:names:tc:opendocument:xmlns:form:1.0" xmlns:script="urn:oasis:names:tc:opendocument:xmlns:script:1.0" xmlns:dom="http://www.w3.org/2001/xml-events" xmlns:xforms="http://www.w3.org/2002/xforms" xmlns:xsd="http://www.w3.org/2001/XMLSchema" office:version="1.2">
+<office:document-content xmlns:presentation="urn:oasis:names:tc:opendocument:xmlns:presentation:1.0" xmlns:css3t="http://www.w3.org/TR/css3-text/" xmlns:grddl="http://www.w3.org/2003/g/data-view#" xmlns:xhtml="http://www.w3.org/1999/xhtml" xmlns:formx="urn:openoffice:names:experimental:ooxml-odf-interop:xmlns:form:1.0" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:rpt="http://openoffice.org/2005/report" xmlns:dc="http://purl.org/dc/elements/1.1/" xmlns:chart="urn:oasis:names:tc:opendocument:xmlns:chart:1.0" xmlns:svg="urn:oasis:names:tc:opendocument:xmlns:svg-compatible:1.0" xmlns:draw="urn:oasis:names:tc:opendocument:xmlns:drawing:1.0" xmlns:text="urn:oasis:names:tc:opendocument:xmlns:text:1.0" xmlns:oooc="http://openoffice.org/2004/calc" xmlns:style="urn:oasis:names:tc:opendocument:xmlns:style:1.0" xmlns:ooow="http://openoffice.org/2004/writer" xmlns:meta="urn:oasis:names:tc:opendocument:xmlns:meta:1.0" xmlns:xlink="http://www.w3.org/1999/xlink" xmlns:fo="urn:oasis:names:tc:opendocument:xmlns:xsl-fo-compatible:1.0" xmlns:ooo="http://openoffice.org/2004/office" xmlns:office="urn:oasis:names:tc:opendocument:xmlns:office:1.0" xmlns:dr3d="urn:oasis:names:tc:opendocument:xmlns:dr3d:1.0" xmlns:table="urn:oasis:names:tc:opendocument:xmlns:table:1.0" xmlns:number="urn:oasis:names:tc:opendocument:xmlns:datastyle:1.0" xmlns:of="urn:oasis:names:tc:opendocument:xmlns:of:1.2" xmlns:calcext="urn:org:documentfoundation:names:experimental:calc:xmlns:calcext:1.0" xmlns:tableooo="http://openoffice.org/2009/table" xmlns:drawooo="http://openoffice.org/2010/draw" xmlns:loext="urn:org:documentfoundation:names:experimental:office:xmlns:loext:1.0" xmlns:dom="http://www.w3.org/2001/xml-events" xmlns:field="urn:openoffice:names:experimental:ooo-ms-interop:xmlns:field:1.0" xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:math="http://www.w3.org/1998/Math/MathML" xmlns:form="urn:oasis:names:tc:opendocument:xmlns:form:1.0" xmlns:script="urn:oasis:names:tc:opendocument:xmlns:script:1.0" xmlns:xforms="http://www.w3.org/2002/xforms" office:version="1.3">
   <office:scripts/>
   <office:font-face-decls>
     <style:font-face style:name="Liberation Sans" svg:font-family="'Liberation Sans'" style:font-family-generic="swiss" style:font-pitch="variable"/>
+    <style:font-face style:name="FreeSans" svg:font-family="FreeSans" style:font-family-generic="system" style:font-pitch="variable"/>
     <style:font-face style:name="Mangal" svg:font-family="Mangal" style:font-family-generic="system" style:font-pitch="variable"/>
     <style:font-face style:name="Microsoft YaHei" svg:font-family="'Microsoft YaHei'" style:font-family-generic="system" style:font-pitch="variable"/>
     <style:font-face style:name="Noto Sans CJK SC" svg:font-family="'Noto Sans CJK SC'" style:font-family-generic="system" style:font-pitch="variable"/>
-    <style:font-face style:name="Noto Sans Devanagari" svg:font-family="'Noto Sans Devanagari'" style:font-family-generic="system" style:font-pitch="variable"/>
     <style:font-face style:name="Segoe UI" svg:font-family="'Segoe UI'" style:font-family-generic="system" style:font-pitch="variable"/>
     <style:font-face style:name="Tahoma" svg:font-family="Tahoma" style:font-family-generic="system" style:font-pitch="variable"/>
   </office:font-face-decls>
   <office:automatic-styles>
     <style:style style:name="co1" style:family="table-column">
-      <style:table-column-properties fo:break-before="auto" style:column-width="0.889in"/>
+      <style:table-column-properties fo:break-before="auto" style:column-width="2.258cm"/>
     </style:style>
     <style:style style:name="ro1" style:family="table-row">
-      <style:table-row-properties style:row-height="0.178in" fo:break-before="auto" style:use-optimal-row-height="true"/>
+      <style:table-row-properties style:row-height="0.452cm" fo:break-before="auto" style:use-optimal-row-height="true"/>
     </style:style>
     <style:style style:name="ta1" style:family="table" style:master-page-name="Default">
       <style:table-properties table:display="true" style:writing-mode="lr-tb"/>
@@ -70,10 +70,10 @@
 </file>
 
 <file path=meta.xml><?xml version="1.0" encoding="utf-8"?>
-<office:document-meta xmlns:grddl="http://www.w3.org/2003/g/data-view#" xmlns:meta="urn:oasis:names:tc:opendocument:xmlns:meta:1.0" xmlns:xlink="http://www.w3.org/1999/xlink" xmlns:dc="http://purl.org/dc/elements/1.1/" xmlns:ooo="http://openoffice.org/2004/office" xmlns:office="urn:oasis:names:tc:opendocument:xmlns:office:1.0" office:version="1.2">
+<office:document-meta xmlns:grddl="http://www.w3.org/2003/g/data-view#" xmlns:meta="urn:oasis:names:tc:opendocument:xmlns:meta:1.0" xmlns:dc="http://purl.org/dc/elements/1.1/" xmlns:xlink="http://www.w3.org/1999/xlink" xmlns:ooo="http://openoffice.org/2004/office" xmlns:office="urn:oasis:names:tc:opendocument:xmlns:office:1.0" office:version="1.3">
   <office:meta>
     <meta:creation-date>2017-10-20T23:41:04.964000000</meta:creation-date>
-    <meta:generator>LibreOffice/6.4.7.2$Linux_X86_64 LibreOffice_project/40$Build-2</meta:generator>
+    <meta:generator>LibreOffice/7.1.2.2$Linux_X86_64 LibreOffice_project/10$Build-2</meta:generator>
     <dc:date>2021-04-21T11:00:36.045089949</dc:date>
     <meta:editing-duration>PT1M33S</meta:editing-duration>
     <meta:editing-cycles>4</meta:editing-cycles>
@@ -83,7 +83,7 @@
 </file>
 
 <file path=settings.xml><?xml version="1.0" encoding="utf-8"?>
-<office:document-settings xmlns:config="urn:oasis:names:tc:opendocument:xmlns:config:1.0" xmlns:xlink="http://www.w3.org/1999/xlink" xmlns:ooo="http://openoffice.org/2004/office" xmlns:office="urn:oasis:names:tc:opendocument:xmlns:office:1.0" office:version="1.2">
+<office:document-settings xmlns:config="urn:oasis:names:tc:opendocument:xmlns:config:1.0" xmlns:xlink="http://www.w3.org/1999/xlink" xmlns:ooo="http://openoffice.org/2004/office" xmlns:office="urn:oasis:names:tc:opendocument:xmlns:office:1.0" office:version="1.3">
   <office:settings>
     <config:config-item-set config:name="ooo:view-settings">
       <config:config-item config:name="VisibleAreaTop" config:type="int">0</config:config-item>
@@ -114,7 +114,7 @@
             </config:config-item-map-entry>
           </config:config-item-map-named>
           <config:config-item config:name="ActiveTable" config:type="string">Sheet1</config:config-item>
-          <config:config-item config:name="HorizontalScrollbarWidth" config:type="int">1298</config:config-item>
+          <config:config-item config:name="HorizontalScrollbarWidth" config:type="int">1857</config:config-item>
           <config:config-item config:name="ZoomType" config:type="short">0</config:config-item>
           <config:config-item config:name="ZoomValue" config:type="int">100</config:config-item>
           <config:config-item config:name="PageViewZoomValue" config:type="int">60</config:config-item>
@@ -151,7 +151,7 @@
       <config:config-item config:name="HasColumnRowHeaders" config:type="boolean">true</config:config-item>
       <config:config-item config:name="ShowNotes" config:type="boolean">true</config:config-item>
       <config:config-item config:name="HasSheetTabs" config:type="boolean">true</config:config-item>
-      <config:config-item config:name="PrinterSetup" config:type="base64Binary">owH+/0dlbmVyaWMgUHJpbnRlcgAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAU0dFTlBSVAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAWAAMAxAAAAAAAAAAIAFZUAAAkbQAASm9iRGF0YSAxCnByaW50ZXI9R2VuZXJpYyBQcmludGVyCm9yaWVudGF0aW9uPVBvcnRyYWl0CmNvcGllcz0xCmNvbGxhdGU9ZmFsc2UKbWFyZ2luZGFqdXN0bWVudD0wLDAsMCwwCmNvbG9yZGVwdGg9MjQKcHNsZXZlbD0wCnBkZmRldmljZT0xCmNvbG9yZGV2aWNlPTAKUFBEQ29udGV4RGF0YQpEdXBsZXg6Tm9uZQBQYWdlU2l6ZTpMZXR0ZXIAABIAQ09NUEFUX0RVUExFWF9NT0RFDwBEdXBsZXhNb2RlOjpPZmY=</config:config-item>
+      <config:config-item config:name="PrinterSetup" config:type="base64Binary">owH+/0dlbmVyaWMgUHJpbnRlcgAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAU0dFTlBSVAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAWAAMAxAAAAAAAAAAIAFZUAAAkbQAASm9iRGF0YSAxCnByaW50ZXI9R2VuZXJpYyBQcmludGVyCm9yaWVudGF0aW9uPVBvcnRyYWl0CmNvcGllcz0xCmNvbGxhdGU9ZmFsc2UKbWFyZ2luZGFqdXN0bWVudD0wLDAsMCwwCmNvbG9yZGVwdGg9MjQKcHNsZXZlbD0wCnBkZmRldmljZT0xCmNvbG9yZGV2aWNlPTAKUFBEQ29udGV4RGF0YQpQYWdlU2l6ZTpMZXR0ZXIARHVwbGV4Ok5vbmUAABIAQ09NUEFUX0RVUExFWF9NT0RFDwBEdXBsZXhNb2RlOjpPZmY=</config:config-item>
       <config:config-item config:name="RasterResolutionX" config:type="int">1270</config:config-item>
       <config:config-item config:name="SyntaxStringRef" config:type="short">7</config:config-item>
       <config:config-item config:name="RasterIsVisible" config:type="boolean">false</config:config-item>
@@ -175,25 +175,30 @@
       <config:config-item config:name="UpdateFromTemplate" config:type="boolean">true</config:config-item>
       <config:config-item config:name="IsDocumentShared" config:type="boolean">false</config:config-item>
       <config:config-item config:name="AllowPrintJobCancel" config:type="boolean">true</config:config-item>
+      <config:config-item-map-named config:name="ScriptConfiguration">
+        <config:config-item-map-entry config:name="Sheet1">
+          <config:config-item config:name="CodeName" config:type="string">Sheet1</config:config-item>
+        </config:config-item-map-entry>
+      </config:config-item-map-named>
     </config:config-item-set>
   </office:settings>
 </office:document-settings>
 </file>
 
 <file path=styles.xml><?xml version="1.0" encoding="utf-8"?>
-<office:document-styles xmlns:presentation="urn:oasis:names:tc:opendocument:xmlns:presentation:1.0" xmlns:css3t="http://www.w3.org/TR/css3-text/" xmlns:chart="urn:oasis:names:tc:opendocument:xmlns:chart:1.0" xmlns:svg="urn:oasis:names:tc:opendocument:xmlns:svg-compatible:1.0" xmlns:draw="urn:oasis:names:tc:opendocument:xmlns:drawing:1.0" xmlns:rpt="http://openoffice.org/2005/report" xmlns:text="urn:oasis:names:tc:opendocument:xmlns:text:1.0" xmlns:style="urn:oasis:names:tc:opendocument:xmlns:style:1.0" xmlns:meta="urn:oasis:names:tc:opendocument:xmlns:meta:1.0" xmlns:xlink="http://www.w3.org/1999/xlink" xmlns:xhtml="http://www.w3.org/1999/xhtml" xmlns:fo="urn:oasis:names:tc:opendocument:xmlns:xsl-fo-compatible:1.0" xmlns:of="urn:oasis:names:tc:opendocument:xmlns:of:1.2" xmlns:dc="http://purl.org/dc/elements/1.1/" xmlns:grddl="http://www.w3.org/2003/g/data-view#" xmlns:ooo="http://openoffice.org/2004/office" xmlns:dr3d="urn:oasis:names:tc:opendocument:xmlns:dr3d:1.0" xmlns:calcext="urn:org:documentfoundation:names:experimental:calc:xmlns:calcext:1.0" xmlns:drawooo="http://openoffice.org/2010/draw" xmlns:field="urn:openoffice:names:experimental:ooo-ms-interop:xmlns:field:1.0" xmlns:office="urn:oasis:names:tc:opendocument:xmlns:office:1.0" xmlns:table="urn:oasis:names:tc:opendocument:xmlns:table:1.0" xmlns:number="urn:oasis:names:tc:opendocument:xmlns:datastyle:1.0" xmlns:ooow="http://openoffice.org/2004/writer" xmlns:oooc="http://openoffice.org/2004/calc" xmlns:tableooo="http://openoffice.org/2009/table" xmlns:loext="urn:org:documentfoundation:names:experimental:office:xmlns:loext:1.0" xmlns:math="http://www.w3.org/1998/Math/MathML" xmlns:form="urn:oasis:names:tc:opendocument:xmlns:form:1.0" xmlns:script="urn:oasis:names:tc:opendocument:xmlns:script:1.0" xmlns:dom="http://www.w3.org/2001/xml-events" office:version="1.2">
+<office:document-styles xmlns:presentation="urn:oasis:names:tc:opendocument:xmlns:presentation:1.0" xmlns:css3t="http://www.w3.org/TR/css3-text/" xmlns:rpt="http://openoffice.org/2005/report" xmlns:dc="http://purl.org/dc/elements/1.1/" xmlns:chart="urn:oasis:names:tc:opendocument:xmlns:chart:1.0" xmlns:svg="urn:oasis:names:tc:opendocument:xmlns:svg-compatible:1.0" xmlns:draw="urn:oasis:names:tc:opendocument:xmlns:drawing:1.0" xmlns:text="urn:oasis:names:tc:opendocument:xmlns:text:1.0" xmlns:oooc="http://openoffice.org/2004/calc" xmlns:style="urn:oasis:names:tc:opendocument:xmlns:style:1.0" xmlns:ooow="http://openoffice.org/2004/writer" xmlns:meta="urn:oasis:names:tc:opendocument:xmlns:meta:1.0" xmlns:xlink="http://www.w3.org/1999/xlink" xmlns:fo="urn:oasis:names:tc:opendocument:xmlns:xsl-fo-compatible:1.0" xmlns:ooo="http://openoffice.org/2004/office" xmlns:office="urn:oasis:names:tc:opendocument:xmlns:office:1.0" xmlns:dr3d="urn:oasis:names:tc:opendocument:xmlns:dr3d:1.0" xmlns:table="urn:oasis:names:tc:opendocument:xmlns:table:1.0" xmlns:number="urn:oasis:names:tc:opendocument:xmlns:datastyle:1.0" xmlns:of="urn:oasis:names:tc:opendocument:xmlns:of:1.2" xmlns:calcext="urn:org:documentfoundation:names:experimental:calc:xmlns:calcext:1.0" xmlns:tableooo="http://openoffice.org/2009/table" xmlns:drawooo="http://openoffice.org/2010/draw" xmlns:grddl="http://www.w3.org/2003/g/data-view#" xmlns:loext="urn:org:documentfoundation:names:experimental:office:xmlns:loext:1.0" xmlns:dom="http://www.w3.org/2001/xml-events" xmlns:field="urn:openoffice:names:experimental:ooo-ms-interop:xmlns:field:1.0" xmlns:math="http://www.w3.org/1998/Math/MathML" xmlns:form="urn:oasis:names:tc:opendocument:xmlns:form:1.0" xmlns:script="urn:oasis:names:tc:opendocument:xmlns:script:1.0" xmlns:xhtml="http://www.w3.org/1999/xhtml" office:version="1.3">
   <office:font-face-decls>
     <style:font-face style:name="Liberation Sans" svg:font-family="'Liberation Sans'" style:font-family-generic="swiss" style:font-pitch="variable"/>
+    <style:font-face style:name="FreeSans" svg:font-family="FreeSans" style:font-family-generic="system" style:font-pitch="variable"/>
     <style:font-face style:name="Mangal" svg:font-family="Mangal" style:font-family-generic="system" style:font-pitch="variable"/>
     <style:font-face style:name="Microsoft YaHei" svg:font-family="'Microsoft YaHei'" style:font-family-generic="system" style:font-pitch="variable"/>
     <style:font-face style:name="Noto Sans CJK SC" svg:font-family="'Noto Sans CJK SC'" style:font-family-generic="system" style:font-pitch="variable"/>
-    <style:font-face style:name="Noto Sans Devanagari" svg:font-family="'Noto Sans Devanagari'" style:font-family-generic="system" style:font-pitch="variable"/>
     <style:font-face style:name="Segoe UI" svg:font-family="'Segoe UI'" style:font-family-generic="system" style:font-pitch="variable"/>
     <style:font-face style:name="Tahoma" svg:font-family="Tahoma" style:font-family-generic="system" style:font-pitch="variable"/>
   </office:font-face-decls>
   <office:styles>
     <style:default-style style:family="table-cell">
-      <style:paragraph-properties style:tab-stop-distance="0.5in"/>
+      <style:paragraph-properties style:tab-stop-distance="1.27cm"/>
       <style:text-properties style:font-name="Liberation Sans" fo:language="en" fo:country="US" style:font-name-asian="Segoe UI" style:language-asian="zh" style:country-asian="CN" style:font-name-complex="Tahoma" style:language-complex="hi" style:country-complex="IN"/>
     </style:default-style>
     <number:number-style style:name="N0">
@@ -261,24 +266,27 @@
     </style:style>
   </office:styles>
   <office:automatic-styles>
+    <number:number-style style:name="N2">
+      <number:number number:decimal-places="2" number:min-decimal-places="2" number:min-integer-digits="1"/>
+    </number:number-style>
     <style:page-layout style:name="Mpm1">
       <style:page-layout-properties style:writing-mode="lr-tb"/>
       <style:header-style>
-        <style:header-footer-properties fo:min-height="0.2953in" fo:margin-left="0in" fo:margin-right="0in" fo:margin-bottom="0.0984in"/>
+        <style:header-footer-properties fo:min-height="0.75cm" fo:margin-left="0cm" fo:margin-right="0cm" fo:margin-bottom="0.25cm"/>
       </style:header-style>
       <style:footer-style>
-        <style:header-footer-properties fo:min-height="0.2953in" fo:margin-left="0in" fo:margin-right="0in" fo:margin-top="0.0984in"/>
+        <style:header-footer-properties fo:min-height="0.75cm" fo:margin-left="0cm" fo:margin-right="0cm" fo:margin-top="0.25cm"/>
       </style:footer-style>
     </style:page-layout>
     <style:page-layout style:name="Mpm2">
       <style:page-layout-properties style:writing-mode="lr-tb"/>
       <style:header-style>
-        <style:header-footer-properties fo:min-height="0.2953in" fo:margin-left="0in" fo:margin-right="0in" fo:margin-bottom="0.0984in" fo:border="2.49pt solid #000000" fo:padding="0.0071in" fo:background-color="#c0c0c0">
+        <style:header-footer-properties fo:min-height="0.75cm" fo:margin-left="0cm" fo:margin-right="0cm" fo:margin-bottom="0.25cm" fo:border="2.49pt solid #000000" fo:padding="0.018cm" fo:background-color="#c0c0c0">
           <style:background-image/>
         </style:header-footer-properties>
       </style:header-style>
       <style:footer-style>
-        <style:header-footer-properties fo:min-height="0.2953in" fo:margin-left="0in" fo:margin-right="0in" fo:margin-top="0.0984in" fo:border="2.49pt solid #000000" fo:padding="0.0071in" fo:background-color="#c0c0c0">
+        <style:header-footer-properties fo:min-height="0.75cm" fo:margin-left="0cm" fo:margin-right="0cm" fo:margin-top="0.25cm" fo:border="2.49pt solid #000000" fo:padding="0.018cm" fo:background-color="#c0c0c0">
           <style:background-image/>
         </style:header-footer-properties>
       </style:footer-style>
@@ -313,9 +321,9 @@
         </style:region-left>
         <style:region-right>
           <text:p>
-            <text:date style:data-style-name="N2" text:date-value="2021-04-21">00/00/0000</text:date>
+            <text:date style:data-style-name="N2" text:date-value="2021-04-22">00/00/0000</text:date>
             , 
-            <text:time style:data-style-name="N2" text:time-value="11:00:02.741014498">00:00:00</text:time>
+            <text:time style:data-style-name="N2" text:time-value="14:59:55.654958104">00:00:00</text:time>
           </text:p>
         </style:region-right>
       </style:header>

</xml_diff>